<commit_message>
renamed planetNumber and seed to planetSeed and worldCoord respectively.
</commit_message>
<xml_diff>
--- a/BlockTypes.xlsx
+++ b/BlockTypes.xlsx
@@ -5,17 +5,18 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LDPlay Asset Source Files\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LDPlay\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49038C9B-E6E9-4494-AA60-05F8C94936C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32199A12-CB74-4614-90EE-7C4AF4E2B269}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{0C60AB3C-82F7-4D00-934D-DF22B92E9E77}"/>
   </bookViews>
   <sheets>
-    <sheet name="BlockType Definitions" sheetId="3" r:id="rId1"/>
-    <sheet name="Colors (source)" sheetId="2" r:id="rId2"/>
-    <sheet name="Colors (filtered)" sheetId="1" r:id="rId3"/>
+    <sheet name="Sheet1" sheetId="4" r:id="rId1"/>
+    <sheet name="BlockType Definitions" sheetId="3" r:id="rId2"/>
+    <sheet name="Colors (source)" sheetId="2" r:id="rId3"/>
+    <sheet name="Colors (filtered)" sheetId="1" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -54,7 +55,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1429" uniqueCount="678">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1432" uniqueCount="681">
   <si>
     <t>0 !COLOUR</t>
   </si>
@@ -2088,6 +2089,15 @@
   </si>
   <si>
     <t>orientations stored in save file to reduce block IDs!!!</t>
+  </si>
+  <si>
+    <t>Each voxel saved as a byte which can hold up to 2^8 = 256 unique block IDs</t>
+  </si>
+  <si>
+    <t>Planet Seed = Int32 which can hold up to 2,147,483,647 unique values</t>
+  </si>
+  <si>
+    <t>World Coord = Int32 which can hold up to 2,147,483,647 unique values</t>
   </si>
 </sst>
 </file>
@@ -2536,11 +2546,39 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{28AE6699-DCF2-4B3F-A092-79CA25402A34}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>679</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>680</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>678</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80F7BB64-65A9-48C6-AE17-93F3C7222BE8}">
   <dimension ref="A1:U258"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O2" sqref="O2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J30" sqref="J30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4606,7 +4644,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{526784A4-4FD2-4332-BC01-24DE6085A369}">
   <dimension ref="A1:G170"/>
   <sheetViews>
@@ -7009,7 +7047,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{692354F1-FBB8-45C8-8585-EA1C7793F7B8}">
   <dimension ref="A1:G86"/>
   <sheetViews>

</xml_diff>